<commit_message>
running bigdata count check
</commit_message>
<xml_diff>
--- a/test/testcases/testcase27_csv_csv_bigdata_match.xlsx
+++ b/test/testcases/testcase27_csv_csv_bigdata_match.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\GitHub\QE_ATF\test\testcases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EE357F-F868-4BB1-A878-0659790A9C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{690D8D0F-D771-44B8-99FD-8B66E517057B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>sourcequerymode</t>
   </si>
@@ -135,10 +135,13 @@
     <t>/app/test/s2t/s2t_27_csv_csv_bigdata_match.xlsx</t>
   </si>
   <si>
-    <t>source_to_target</t>
-  </si>
-  <si>
     <t>testcase27_csv_csv_bigdata_match</t>
+  </si>
+  <si>
+    <t>source_to_stage</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -533,8 +536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +553,7 @@
         <v>11</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -739,14 +742,16 @@
         <v>2</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">

</xml_diff>